<commit_message>
adc_sample: basic working! and tested!
</commit_message>
<xml_diff>
--- a/DOC/pin分配.xlsx
+++ b/DOC/pin分配.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,14 +40,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MCU串口发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MCU串口收</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PA8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -140,14 +132,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>板载绿色LED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>板载红色LED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -176,19 +160,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>USART2_TX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USART2_RX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PA2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PA3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU串口发-usart3_tx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU串口收-usart3_rx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>usart1_tx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>usart1_rx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用途</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tuya</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>板载绿色LED，低亮高灭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>板载红色LED，低亮高灭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC1_CH0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC1_CH4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC1_CH6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC2_CH5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -221,7 +249,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -244,13 +272,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -259,6 +313,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,21 +619,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.1328125" style="1" customWidth="1"/>
     <col min="2" max="3" width="13.73046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.19921875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -587,222 +647,248 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>34</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
@@ -811,23 +897,31 @@
         <v>40</v>
       </c>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F15:F16"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
doc: update pinout doc
</commit_message>
<xml_diff>
--- a/DOC/pin分配.xlsx
+++ b/DOC/pin分配.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -208,15 +208,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ADC1_CH6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC2_CH5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSK控制的慢1/4相位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ADC1_CH4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ADC1_CH6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADC2_CH5</t>
+    <t>PWM输出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -249,7 +257,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -272,39 +280,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -314,10 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -619,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -633,7 +612,7 @@
     <col min="5" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -652,8 +631,9 @@
       <c r="F1" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -670,8 +650,9 @@
         <v>7</v>
       </c>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -688,8 +669,9 @@
         <v>18</v>
       </c>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -704,10 +686,11 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>48</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -722,10 +705,11 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>49</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -744,8 +728,9 @@
       <c r="F6" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -761,9 +746,10 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" s="3"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -778,8 +764,9 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -794,8 +781,9 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -810,8 +798,9 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -826,8 +815,9 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -846,8 +836,9 @@
       <c r="F12" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -858,16 +849,19 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>51</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -882,8 +876,9 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -900,8 +895,9 @@
       <c r="F15" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -915,7 +911,8 @@
         <v>41</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
adc_sample: optimise the memory access
</commit_message>
<xml_diff>
--- a/DOC/pin分配.xlsx
+++ b/DOC/pin分配.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -224,7 +224,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PWM输出</t>
+    <t>PWM输出检查口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC采集检查口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>临时功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -600,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -609,7 +617,9 @@
     <col min="1" max="1" width="12.1328125" style="1" customWidth="1"/>
     <col min="2" max="3" width="13.73046875" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.19921875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="1"/>
+    <col min="5" max="6" width="9.06640625" style="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -631,7 +641,9 @@
       <c r="F1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2">
@@ -836,7 +848,9 @@
       <c r="F12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2">

</xml_diff>